<commit_message>
Update Music/Stuart Audio Asset List.xlsx
</commit_message>
<xml_diff>
--- a/Music/Stuart Audio Asset List.xlsx
+++ b/Music/Stuart Audio Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="105">
   <si>
     <t>NAME</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>Tveil_Credits_SB</t>
+  </si>
+  <si>
+    <t>Implemented</t>
   </si>
 </sst>
 </file>
@@ -779,7 +782,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,11 +843,11 @@
       <c r="E3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>36</v>
+      <c r="F3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
@@ -866,11 +869,11 @@
       <c r="E4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
+      <c r="F4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
@@ -892,11 +895,11 @@
       <c r="E5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>36</v>
+      <c r="F5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -918,8 +921,8 @@
       <c r="E6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>36</v>
+      <c r="F6" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>36</v>
@@ -947,8 +950,8 @@
       <c r="E7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
+      <c r="F7" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -976,8 +979,8 @@
       <c r="E8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>36</v>
+      <c r="F8" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>36</v>
@@ -1005,8 +1008,8 @@
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
+      <c r="F9" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>36</v>
@@ -1031,8 +1034,8 @@
       <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
+      <c r="F10" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
@@ -1057,8 +1060,8 @@
       <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>36</v>
+      <c r="F11" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Updating Master Branch Music folder
</commit_message>
<xml_diff>
--- a/Music/Stuart Audio Asset List.xlsx
+++ b/Music/Stuart Audio Asset List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\StuHome\HomeDrive1$\1804801\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\StuHome\HomeDrive1$\1804801\Desktop\Team-X-Masterpiece\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -782,7 +782,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,14 +1491,14 @@
       <c r="D27" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>36</v>
+      <c r="E27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H27" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Updated Audio asset List
</commit_message>
<xml_diff>
--- a/Music/Stuart Audio Asset List.xlsx
+++ b/Music/Stuart Audio Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="107">
   <si>
     <t>NAME</t>
   </si>
@@ -349,11 +349,6 @@
 3 and 2</t>
   </si>
   <si>
-    <t>Awaiting confirmation
-on level theme 
-aesthetic</t>
-  </si>
-  <si>
     <t>Tveil_Lvl_SB</t>
   </si>
   <si>
@@ -364,6 +359,15 @@
   </si>
   <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>Aztec/Mayan Tropes</t>
+  </si>
+  <si>
+    <t>Egyptian/Middle Eastern Tropes</t>
+  </si>
+  <si>
+    <t>Far Eastern/Asian Tropes</t>
   </si>
 </sst>
 </file>
@@ -782,7 +786,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
@@ -844,10 +848,10 @@
         <v>33</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
@@ -858,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -870,10 +874,10 @@
         <v>33</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
@@ -884,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -896,10 +900,10 @@
         <v>33</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -910,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>93</v>
@@ -922,7 +926,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>36</v>
@@ -939,7 +943,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>93</v>
@@ -951,7 +955,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -968,7 +972,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>93</v>
@@ -980,7 +984,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>36</v>
@@ -997,7 +1001,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>77</v>
@@ -1009,7 +1013,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>36</v>
@@ -1023,7 +1027,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>77</v>
@@ -1035,7 +1039,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
@@ -1049,7 +1053,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>77</v>
@@ -1061,7 +1065,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>36</v>
@@ -1075,7 +1079,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>78</v>
@@ -1101,7 +1105,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>79</v>
@@ -1127,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>80</v>
@@ -1138,8 +1142,8 @@
       <c r="E14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>36</v>
+      <c r="F14" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>36</v>
@@ -1156,7 +1160,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>81</v>
@@ -1182,7 +1186,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>82</v>
@@ -1193,11 +1197,11 @@
       <c r="E16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>36</v>
+      <c r="F16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H16" t="s">
         <v>37</v>
@@ -1208,7 +1212,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
         <v>82</v>
@@ -1219,11 +1223,11 @@
       <c r="E17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>36</v>
+      <c r="F17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H17" t="s">
         <v>37</v>
@@ -1234,7 +1238,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>83</v>
@@ -1263,7 +1267,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>84</v>
@@ -1274,8 +1278,8 @@
       <c r="E19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>36</v>
+      <c r="F19" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>36</v>
@@ -1289,7 +1293,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>84</v>
@@ -1318,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>84</v>
@@ -1347,7 +1351,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>85</v>
@@ -1376,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>86</v>
@@ -1402,7 +1406,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>87</v>
@@ -1413,11 +1417,11 @@
       <c r="E24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>36</v>
+      <c r="F24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
@@ -1428,7 +1432,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>88</v>
@@ -1439,8 +1443,8 @@
       <c r="E25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>36</v>
+      <c r="F25" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
@@ -1454,7 +1458,7 @@
         <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>89</v>
@@ -1478,15 +1482,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>100</v>
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>91</v>
@@ -1504,41 +1508,41 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>100</v>
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>36</v>
+      <c r="E28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>100</v>
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>92</v>
@@ -1556,24 +1560,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C30" s="10"/>
       <c r="D30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>36</v>
+      <c r="E30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>36</v>
@@ -1582,24 +1584,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C31" s="10"/>
       <c r="D31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>36</v>
+      <c r="E31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>36</v>
@@ -1608,24 +1608,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C32" s="10"/>
       <c r="D32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>36</v>
+      <c r="E32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>36</v>
@@ -1634,24 +1632,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C33" s="10"/>
       <c r="D33" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>36</v>
+      <c r="E33" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>36</v>
@@ -1660,24 +1656,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C34" s="10"/>
       <c r="D34" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>36</v>
+      <c r="E34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>36</v>
@@ -1686,24 +1680,22 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>100</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C35" s="10"/>
       <c r="D35" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>36</v>
+      <c r="E35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>36</v>

</xml_diff>